<commit_message>
gbif data wrangling for climate regions
</commit_message>
<xml_diff>
--- a/shared analysis files /metafor.xlsx
+++ b/shared analysis files /metafor.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/shared analysis files /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF3966D-3063-6C47-A3F8-CFFA9C1A163D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B9C4A3-2E63-E149-A4A3-036825CEDB16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29080" yWindow="-9980" windowWidth="21860" windowHeight="15400" xr2:uid="{4536B02C-F584-4642-B8E5-0FF5356DC288}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="228">
   <si>
     <t>study_id</t>
   </si>
@@ -707,6 +707,9 @@
   <si>
     <t>n</t>
   </si>
+  <si>
+    <t>Mauremys</t>
+  </si>
 </sst>
 </file>
 
@@ -1068,9 +1071,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCFBC2B-929F-FD41-8C91-75842D1EBA74}">
   <dimension ref="A1:AJ272"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A252" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X3" sqref="X3:X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="X2" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y2" t="s">
         <v>33</v>
@@ -1347,7 +1350,7 @@
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y3" t="s">
         <v>33</v>
@@ -1440,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="X4" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y4" t="s">
         <v>33</v>
@@ -1533,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y5" t="s">
         <v>33</v>
@@ -1626,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="X6" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y6" t="s">
         <v>33</v>
@@ -1719,7 +1722,7 @@
         <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y7" t="s">
         <v>33</v>
@@ -1812,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y8" t="s">
         <v>33</v>
@@ -1905,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="X9" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y9" t="s">
         <v>33</v>
@@ -1998,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="X10" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y10" t="s">
         <v>33</v>
@@ -2091,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="X11" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y11" t="s">
         <v>33</v>
@@ -2184,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="X12" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y12" t="s">
         <v>33</v>
@@ -2277,7 +2280,7 @@
         <v>0</v>
       </c>
       <c r="X13" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y13" t="s">
         <v>33</v>
@@ -2370,7 +2373,7 @@
         <v>0</v>
       </c>
       <c r="X14" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y14" t="s">
         <v>33</v>
@@ -2469,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="X15" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y15" t="s">
         <v>33</v>
@@ -2568,7 +2571,7 @@
         <v>0</v>
       </c>
       <c r="X16" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y16" t="s">
         <v>33</v>
@@ -2667,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="X17" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y17" t="s">
         <v>33</v>
@@ -2766,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="X18" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y18" t="s">
         <v>33</v>
@@ -2859,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="X19" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y19" t="s">
         <v>33</v>
@@ -2958,7 +2961,7 @@
         <v>0</v>
       </c>
       <c r="X20" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y20" t="s">
         <v>33</v>
@@ -3057,7 +3060,7 @@
         <v>0</v>
       </c>
       <c r="X21" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y21" t="s">
         <v>33</v>
@@ -3156,7 +3159,7 @@
         <v>0</v>
       </c>
       <c r="X22" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y22" t="s">
         <v>33</v>
@@ -3255,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="X23" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y23" t="s">
         <v>33</v>
@@ -3354,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="X24" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y24" t="s">
         <v>33</v>
@@ -3447,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="X25" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y25" t="s">
         <v>33</v>
@@ -3546,7 +3549,7 @@
         <v>0</v>
       </c>
       <c r="X26" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y26" t="s">
         <v>33</v>
@@ -3645,7 +3648,7 @@
         <v>0</v>
       </c>
       <c r="X27" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y27" t="s">
         <v>33</v>
@@ -3744,7 +3747,7 @@
         <v>0</v>
       </c>
       <c r="X28" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y28" t="s">
         <v>33</v>
@@ -3843,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="X29" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y29" t="s">
         <v>33</v>
@@ -3942,7 +3945,7 @@
         <v>0</v>
       </c>
       <c r="X30" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y30" t="s">
         <v>33</v>
@@ -4035,7 +4038,7 @@
         <v>0</v>
       </c>
       <c r="X31" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y31" t="s">
         <v>33</v>
@@ -4134,7 +4137,7 @@
         <v>0</v>
       </c>
       <c r="X32" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y32" t="s">
         <v>33</v>
@@ -4233,7 +4236,7 @@
         <v>0</v>
       </c>
       <c r="X33" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y33" t="s">
         <v>33</v>
@@ -4332,7 +4335,7 @@
         <v>0</v>
       </c>
       <c r="X34" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y34" t="s">
         <v>33</v>
@@ -4431,7 +4434,7 @@
         <v>0</v>
       </c>
       <c r="X35" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y35" t="s">
         <v>33</v>
@@ -4530,7 +4533,7 @@
         <v>0</v>
       </c>
       <c r="X36" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="Y36" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
updates to the rmd to remove unnecessary EDA and updating metafor file
</commit_message>
<xml_diff>
--- a/shared analysis files /metafor.xlsx
+++ b/shared analysis files /metafor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/shared analysis files /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1804CB09-5E3B-CD4F-84CB-EC8A5F89F282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{141B151F-8E09-414A-9956-857626E66BAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30020" yWindow="-24840" windowWidth="22780" windowHeight="21480" xr2:uid="{4536B02C-F584-4642-B8E5-0FF5356DC288}"/>
   </bookViews>
@@ -997,7 +997,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R47" sqref="A47:XFD48"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding in column for stressful or not
</commit_message>
<xml_diff>
--- a/shared analysis files /metafor.xlsx
+++ b/shared analysis files /metafor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/shared analysis files /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{141B151F-8E09-414A-9956-857626E66BAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{301DCB65-9442-384B-B095-1BB3A3F429D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30020" yWindow="-24840" windowWidth="22780" windowHeight="21480" xr2:uid="{4536B02C-F584-4642-B8E5-0FF5356DC288}"/>
+    <workbookView xWindow="28820" yWindow="-24920" windowWidth="25220" windowHeight="21480" xr2:uid="{4536B02C-F584-4642-B8E5-0FF5356DC288}"/>
   </bookViews>
   <sheets>
     <sheet name="metafor" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="207">
   <si>
     <t>study_id</t>
   </si>
@@ -640,16 +640,29 @@
   </si>
   <si>
     <t>Mauremys</t>
+  </si>
+  <si>
+    <t>stressful</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -675,10 +688,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -993,16 +1007,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCFBC2B-929F-FD41-8C91-75842D1EBA74}">
-  <dimension ref="A1:AJ158"/>
+  <dimension ref="A1:AK158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="AK159" sqref="AK159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1111,8 +1124,11 @@
       <c r="AJ1" t="s">
         <v>201</v>
       </c>
+      <c r="AK1" t="s">
+        <v>205</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1144,7 +1160,7 @@
         <v>31</v>
       </c>
       <c r="L2">
-        <f>K2-J2</f>
+        <f t="shared" ref="L2:L33" si="0">K2-J2</f>
         <v>6</v>
       </c>
       <c r="M2">
@@ -1204,8 +1220,11 @@
       <c r="AJ2" t="s">
         <v>202</v>
       </c>
+      <c r="AK2" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1237,7 +1256,7 @@
         <v>34</v>
       </c>
       <c r="L3">
-        <f>K3-J3</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M3">
@@ -1297,8 +1316,11 @@
       <c r="AJ3" t="s">
         <v>202</v>
       </c>
+      <c r="AK3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1330,7 +1352,7 @@
         <v>31</v>
       </c>
       <c r="L4">
-        <f>K4-J4</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M4">
@@ -1390,8 +1412,11 @@
       <c r="AJ4" t="s">
         <v>202</v>
       </c>
+      <c r="AK4" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1423,7 +1448,7 @@
         <v>34</v>
       </c>
       <c r="L5">
-        <f>K5-J5</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M5">
@@ -1483,8 +1508,11 @@
       <c r="AJ5" t="s">
         <v>202</v>
       </c>
+      <c r="AK5" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1516,7 +1544,7 @@
         <v>31</v>
       </c>
       <c r="L6">
-        <f>K6-J6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M6">
@@ -1576,8 +1604,11 @@
       <c r="AJ6" t="s">
         <v>202</v>
       </c>
+      <c r="AK6" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1609,7 +1640,7 @@
         <v>34</v>
       </c>
       <c r="L7">
-        <f>K7-J7</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M7">
@@ -1669,8 +1700,11 @@
       <c r="AJ7" t="s">
         <v>202</v>
       </c>
+      <c r="AK7" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1702,7 +1736,7 @@
         <v>31</v>
       </c>
       <c r="L8">
-        <f>K8-J8</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M8">
@@ -1762,8 +1796,11 @@
       <c r="AJ8" t="s">
         <v>202</v>
       </c>
+      <c r="AK8" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1795,7 +1832,7 @@
         <v>34</v>
       </c>
       <c r="L9">
-        <f>K9-J9</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M9">
@@ -1855,8 +1892,11 @@
       <c r="AJ9" t="s">
         <v>202</v>
       </c>
+      <c r="AK9" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1888,7 +1928,7 @@
         <v>31</v>
       </c>
       <c r="L10">
-        <f>K10-J10</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M10">
@@ -1948,8 +1988,11 @@
       <c r="AJ10" t="s">
         <v>202</v>
       </c>
+      <c r="AK10" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1981,7 +2024,7 @@
         <v>34</v>
       </c>
       <c r="L11">
-        <f>K11-J11</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M11">
@@ -2041,8 +2084,11 @@
       <c r="AJ11" t="s">
         <v>202</v>
       </c>
+      <c r="AK11" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
@@ -2074,7 +2120,7 @@
         <v>31</v>
       </c>
       <c r="L12">
-        <f>K12-J12</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M12">
@@ -2134,8 +2180,11 @@
       <c r="AJ12" t="s">
         <v>202</v>
       </c>
+      <c r="AK12" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
@@ -2167,7 +2216,7 @@
         <v>34</v>
       </c>
       <c r="L13">
-        <f>K13-J13</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M13">
@@ -2227,8 +2276,11 @@
       <c r="AJ13" t="s">
         <v>202</v>
       </c>
+      <c r="AK13" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4</v>
       </c>
@@ -2260,7 +2312,7 @@
         <v>31</v>
       </c>
       <c r="L14">
-        <f>K14-J14</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M14">
@@ -2326,8 +2378,11 @@
       <c r="AJ14" t="s">
         <v>202</v>
       </c>
+      <c r="AK14" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
@@ -2359,7 +2414,7 @@
         <v>34</v>
       </c>
       <c r="L15">
-        <f>K15-J15</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M15">
@@ -2425,8 +2480,11 @@
       <c r="AJ15" t="s">
         <v>202</v>
       </c>
+      <c r="AK15" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
@@ -2458,7 +2516,7 @@
         <v>31</v>
       </c>
       <c r="L16">
-        <f>K16-J16</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M16">
@@ -2524,8 +2582,11 @@
       <c r="AJ16" t="s">
         <v>202</v>
       </c>
+      <c r="AK16" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2557,7 +2618,7 @@
         <v>34</v>
       </c>
       <c r="L17">
-        <f>K17-J17</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M17">
@@ -2623,8 +2684,11 @@
       <c r="AJ17" t="s">
         <v>202</v>
       </c>
+      <c r="AK17" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2659,7 +2723,7 @@
         <v>18.5</v>
       </c>
       <c r="L18">
-        <f>K18-J18</f>
+        <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
       <c r="M18">
@@ -2714,7 +2778,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2749,7 +2813,7 @@
         <v>24.5</v>
       </c>
       <c r="L19">
-        <f>K19-J19</f>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="M19">
@@ -2804,7 +2868,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2839,7 +2903,7 @@
         <v>27.5</v>
       </c>
       <c r="L20">
-        <f>K20-J20</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="M20">
@@ -2894,7 +2958,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2929,7 +2993,7 @@
         <v>30</v>
       </c>
       <c r="L21">
-        <f>K21-J21</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="M21">
@@ -2984,7 +3048,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3019,7 +3083,7 @@
         <v>30.5</v>
       </c>
       <c r="L22">
-        <f>K22-J22</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="M22">
@@ -3074,7 +3138,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -3109,7 +3173,7 @@
         <v>36.5</v>
       </c>
       <c r="L23">
-        <f>K23-J23</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="M23">
@@ -3164,7 +3228,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -3199,7 +3263,7 @@
         <v>36.5</v>
       </c>
       <c r="L24">
-        <f>K24-J24</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="M24">
@@ -3254,7 +3318,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -3289,7 +3353,7 @@
         <v>36.5</v>
       </c>
       <c r="L25">
-        <f>K25-J25</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M25">
@@ -3344,7 +3408,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -3379,7 +3443,7 @@
         <v>36.5</v>
       </c>
       <c r="L26">
-        <f>K26-J26</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="M26">
@@ -3431,7 +3495,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -3466,7 +3530,7 @@
         <v>33</v>
       </c>
       <c r="L27">
-        <f>K27-J27</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="M27">
@@ -3532,8 +3596,11 @@
       <c r="AJ27" t="s">
         <v>202</v>
       </c>
+      <c r="AK27" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -3568,7 +3635,7 @@
         <v>33</v>
       </c>
       <c r="L28">
-        <f>K28-J28</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="M28">
@@ -3634,8 +3701,11 @@
       <c r="AJ28" t="s">
         <v>202</v>
       </c>
+      <c r="AK28" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -3670,7 +3740,7 @@
         <v>33</v>
       </c>
       <c r="L29">
-        <f>K29-J29</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="M29">
@@ -3736,8 +3806,11 @@
       <c r="AJ29" t="s">
         <v>202</v>
       </c>
+      <c r="AK29" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="30" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -3772,7 +3845,7 @@
         <v>33</v>
       </c>
       <c r="L30">
-        <f>K30-J30</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="M30">
@@ -3838,8 +3911,11 @@
       <c r="AJ30" t="s">
         <v>202</v>
       </c>
+      <c r="AK30" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -3874,7 +3950,7 @@
         <v>33</v>
       </c>
       <c r="L31">
-        <f>K31-J31</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="M31">
@@ -3940,8 +4016,11 @@
       <c r="AJ31" t="s">
         <v>202</v>
       </c>
+      <c r="AK31" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -3976,7 +4055,7 @@
         <v>33</v>
       </c>
       <c r="L32">
-        <f>K32-J32</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="M32">
@@ -4042,8 +4121,11 @@
       <c r="AJ32" t="s">
         <v>202</v>
       </c>
+      <c r="AK32" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
@@ -4078,7 +4160,7 @@
         <v>33</v>
       </c>
       <c r="L33">
-        <f>K33-J33</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="M33">
@@ -4144,8 +4226,11 @@
       <c r="AJ33" t="s">
         <v>202</v>
       </c>
+      <c r="AK33" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2</v>
       </c>
@@ -4180,7 +4265,7 @@
         <v>33</v>
       </c>
       <c r="L34">
-        <f>K34-J34</f>
+        <f t="shared" ref="L34:L65" si="1">K34-J34</f>
         <v>10</v>
       </c>
       <c r="M34">
@@ -4246,8 +4331,11 @@
       <c r="AJ34" t="s">
         <v>202</v>
       </c>
+      <c r="AK34" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="35" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -4279,7 +4367,7 @@
         <v>30</v>
       </c>
       <c r="L35">
-        <f>K35-J35</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M35">
@@ -4333,8 +4421,11 @@
       <c r="AJ35" t="s">
         <v>202</v>
       </c>
+      <c r="AK35" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2</v>
       </c>
@@ -4366,7 +4457,7 @@
         <v>30</v>
       </c>
       <c r="L36">
-        <f>K36-J36</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M36">
@@ -4420,8 +4511,11 @@
       <c r="AJ36" t="s">
         <v>202</v>
       </c>
+      <c r="AK36" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -4453,7 +4547,7 @@
         <v>30</v>
       </c>
       <c r="L37">
-        <f>K37-J37</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M37">
@@ -4507,8 +4601,11 @@
       <c r="AJ37" t="s">
         <v>202</v>
       </c>
+      <c r="AK37" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -4540,7 +4637,7 @@
         <v>30</v>
       </c>
       <c r="L38">
-        <f>K38-J38</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M38">
@@ -4594,8 +4691,11 @@
       <c r="AJ38" t="s">
         <v>202</v>
       </c>
+      <c r="AK38" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -4627,7 +4727,7 @@
         <v>30</v>
       </c>
       <c r="L39">
-        <f>K39-J39</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M39">
@@ -4681,8 +4781,11 @@
       <c r="AJ39" t="s">
         <v>202</v>
       </c>
+      <c r="AK39" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
@@ -4714,7 +4817,7 @@
         <v>30</v>
       </c>
       <c r="L40">
-        <f>K40-J40</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M40">
@@ -4768,8 +4871,11 @@
       <c r="AJ40" t="s">
         <v>202</v>
       </c>
+      <c r="AK40" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3</v>
       </c>
@@ -4801,7 +4907,7 @@
         <v>30</v>
       </c>
       <c r="L41">
-        <f>K41-J41</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M41">
@@ -4855,8 +4961,11 @@
       <c r="AJ41" t="s">
         <v>202</v>
       </c>
+      <c r="AK41" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>4</v>
       </c>
@@ -4888,7 +4997,7 @@
         <v>30</v>
       </c>
       <c r="L42">
-        <f>K42-J42</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M42">
@@ -4942,8 +5051,11 @@
       <c r="AJ42" t="s">
         <v>202</v>
       </c>
+      <c r="AK42" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -4975,7 +5087,7 @@
         <v>30</v>
       </c>
       <c r="L43">
-        <f>K43-J43</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M43">
@@ -5029,8 +5141,11 @@
       <c r="AJ43" t="s">
         <v>202</v>
       </c>
+      <c r="AK43" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
@@ -5062,7 +5177,7 @@
         <v>30</v>
       </c>
       <c r="L44">
-        <f>K44-J44</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M44">
@@ -5116,8 +5231,11 @@
       <c r="AJ44" t="s">
         <v>202</v>
       </c>
+      <c r="AK44" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>4</v>
       </c>
@@ -5149,7 +5267,7 @@
         <v>30</v>
       </c>
       <c r="L45">
-        <f>K45-J45</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M45">
@@ -5203,8 +5321,11 @@
       <c r="AJ45" t="s">
         <v>202</v>
       </c>
+      <c r="AK45" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -5236,7 +5357,7 @@
         <v>30</v>
       </c>
       <c r="L46">
-        <f>K46-J46</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M46">
@@ -5290,8 +5411,11 @@
       <c r="AJ46" t="s">
         <v>202</v>
       </c>
+      <c r="AK46" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
@@ -5326,7 +5450,7 @@
         <v>28</v>
       </c>
       <c r="L47">
-        <f>K47-J47</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M47">
@@ -5380,8 +5504,11 @@
       <c r="AJ47" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK47" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1</v>
       </c>
@@ -5416,7 +5543,7 @@
         <v>28</v>
       </c>
       <c r="L48">
-        <f>K48-J48</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M48">
@@ -5470,8 +5597,11 @@
       <c r="AJ48" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK48" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2</v>
       </c>
@@ -5506,7 +5636,7 @@
         <v>28</v>
       </c>
       <c r="L49">
-        <f>K49-J49</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M49">
@@ -5560,8 +5690,11 @@
       <c r="AJ49" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK49" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -5596,7 +5729,7 @@
         <v>28</v>
       </c>
       <c r="L50">
-        <f>K50-J50</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M50">
@@ -5650,8 +5783,11 @@
       <c r="AJ50" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK50" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3</v>
       </c>
@@ -5686,7 +5822,7 @@
         <v>28</v>
       </c>
       <c r="L51">
-        <f>K51-J51</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M51">
@@ -5740,8 +5876,11 @@
       <c r="AJ51" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK51" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3</v>
       </c>
@@ -5776,7 +5915,7 @@
         <v>28</v>
       </c>
       <c r="L52">
-        <f>K52-J52</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M52">
@@ -5830,8 +5969,11 @@
       <c r="AJ52" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK52" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>4</v>
       </c>
@@ -5866,7 +6008,7 @@
         <v>28</v>
       </c>
       <c r="L53">
-        <f>K53-J53</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M53">
@@ -5920,8 +6062,11 @@
       <c r="AJ53" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK53" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>4</v>
       </c>
@@ -5956,7 +6101,7 @@
         <v>28</v>
       </c>
       <c r="L54">
-        <f>K54-J54</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M54">
@@ -6010,8 +6155,11 @@
       <c r="AJ54" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK54" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>5</v>
       </c>
@@ -6046,7 +6194,7 @@
         <v>28</v>
       </c>
       <c r="L55">
-        <f>K55-J55</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M55">
@@ -6100,8 +6248,11 @@
       <c r="AJ55" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK55" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>5</v>
       </c>
@@ -6136,7 +6287,7 @@
         <v>28</v>
       </c>
       <c r="L56">
-        <f>K56-J56</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M56">
@@ -6190,8 +6341,11 @@
       <c r="AJ56" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK56" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>6</v>
       </c>
@@ -6226,7 +6380,7 @@
         <v>28</v>
       </c>
       <c r="L57">
-        <f>K57-J57</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M57">
@@ -6280,8 +6434,11 @@
       <c r="AJ57" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK57" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>6</v>
       </c>
@@ -6316,7 +6473,7 @@
         <v>28</v>
       </c>
       <c r="L58">
-        <f>K58-J58</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M58">
@@ -6370,8 +6527,11 @@
       <c r="AJ58" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK58" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1</v>
       </c>
@@ -6403,7 +6563,7 @@
         <v>32</v>
       </c>
       <c r="L59">
-        <f>K59-J59</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M59">
@@ -6466,8 +6626,11 @@
       <c r="AJ59" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK59" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -6499,7 +6662,7 @@
         <v>32</v>
       </c>
       <c r="L60">
-        <f>K60-J60</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M60">
@@ -6562,8 +6725,11 @@
       <c r="AJ60" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK60" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2</v>
       </c>
@@ -6595,7 +6761,7 @@
         <v>32</v>
       </c>
       <c r="L61">
-        <f>K61-J61</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M61">
@@ -6661,8 +6827,11 @@
       <c r="AJ61" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK61" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2</v>
       </c>
@@ -6694,7 +6863,7 @@
         <v>32</v>
       </c>
       <c r="L62">
-        <f>K62-J62</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M62">
@@ -6760,8 +6929,11 @@
       <c r="AJ62" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK62" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1</v>
       </c>
@@ -6793,7 +6965,7 @@
         <v>33</v>
       </c>
       <c r="L63">
-        <f>K63-J63</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="M63">
@@ -6853,8 +7025,11 @@
       <c r="AJ63" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK63" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2</v>
       </c>
@@ -6886,7 +7061,7 @@
         <v>33</v>
       </c>
       <c r="L64">
-        <f>K64-J64</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="M64">
@@ -6946,8 +7121,11 @@
       <c r="AJ64" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK64" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>3</v>
       </c>
@@ -6979,7 +7157,7 @@
         <v>33</v>
       </c>
       <c r="L65">
-        <f>K65-J65</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="M65">
@@ -7039,8 +7217,11 @@
       <c r="AJ65" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK65" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>4</v>
       </c>
@@ -7072,7 +7253,7 @@
         <v>33</v>
       </c>
       <c r="L66">
-        <f>K66-J66</f>
+        <f t="shared" ref="L66:L97" si="2">K66-J66</f>
         <v>4</v>
       </c>
       <c r="M66">
@@ -7132,8 +7313,11 @@
       <c r="AJ66" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK66" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>5</v>
       </c>
@@ -7165,7 +7349,7 @@
         <v>33</v>
       </c>
       <c r="L67">
-        <f>K67-J67</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M67">
@@ -7225,8 +7409,11 @@
       <c r="AJ67" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK67" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1</v>
       </c>
@@ -7258,7 +7445,7 @@
         <v>33</v>
       </c>
       <c r="L68">
-        <f>K68-J68</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M68">
@@ -7318,8 +7505,11 @@
       <c r="AJ68" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK68" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2</v>
       </c>
@@ -7351,7 +7541,7 @@
         <v>33</v>
       </c>
       <c r="L69">
-        <f>K69-J69</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M69">
@@ -7411,8 +7601,11 @@
       <c r="AJ69" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK69" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>3</v>
       </c>
@@ -7444,7 +7637,7 @@
         <v>33</v>
       </c>
       <c r="L70">
-        <f>K70-J70</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M70">
@@ -7504,8 +7697,11 @@
       <c r="AJ70" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK70" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>4</v>
       </c>
@@ -7537,7 +7733,7 @@
         <v>33</v>
       </c>
       <c r="L71">
-        <f>K71-J71</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M71">
@@ -7597,8 +7793,11 @@
       <c r="AJ71" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK71" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>5</v>
       </c>
@@ -7630,7 +7829,7 @@
         <v>33</v>
       </c>
       <c r="L72">
-        <f>K72-J72</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M72">
@@ -7690,8 +7889,11 @@
       <c r="AJ72" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK72" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1</v>
       </c>
@@ -7723,7 +7925,7 @@
         <v>34</v>
       </c>
       <c r="L73">
-        <f>K73-J73</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M73">
@@ -7783,8 +7985,11 @@
       <c r="AJ73" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK73" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2</v>
       </c>
@@ -7816,7 +8021,7 @@
         <v>34</v>
       </c>
       <c r="L74">
-        <f>K74-J74</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M74">
@@ -7876,8 +8081,11 @@
       <c r="AJ74" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK74" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>3</v>
       </c>
@@ -7909,7 +8117,7 @@
         <v>34</v>
       </c>
       <c r="L75">
-        <f>K75-J75</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M75">
@@ -7969,8 +8177,11 @@
       <c r="AJ75" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK75" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>4</v>
       </c>
@@ -8002,7 +8213,7 @@
         <v>34</v>
       </c>
       <c r="L76">
-        <f>K76-J76</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M76">
@@ -8062,8 +8273,11 @@
       <c r="AJ76" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK76" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>5</v>
       </c>
@@ -8095,7 +8309,7 @@
         <v>34</v>
       </c>
       <c r="L77">
-        <f>K77-J77</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M77">
@@ -8155,8 +8369,11 @@
       <c r="AJ77" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK77" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="78" spans="1:36" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:37" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>1</v>
       </c>
@@ -8188,7 +8405,7 @@
         <v>30</v>
       </c>
       <c r="L78">
-        <f>K78-J78</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="M78" s="1">
@@ -8236,8 +8453,11 @@
       <c r="AJ78" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK78" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="79" spans="1:36" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:37" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>1</v>
       </c>
@@ -8269,7 +8489,7 @@
         <v>35</v>
       </c>
       <c r="L79">
-        <f>K79-J79</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M79" s="1">
@@ -8317,8 +8537,11 @@
       <c r="AJ79" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK79" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1</v>
       </c>
@@ -8353,7 +8576,7 @@
         <v>23</v>
       </c>
       <c r="L80">
-        <f>K80-J80</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="M80">
@@ -8407,8 +8630,11 @@
       <c r="AJ80" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK80" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2</v>
       </c>
@@ -8443,7 +8669,7 @@
         <v>23</v>
       </c>
       <c r="L81">
-        <f>K81-J81</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="M81">
@@ -8497,8 +8723,11 @@
       <c r="AJ81" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK81" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>3</v>
       </c>
@@ -8533,7 +8762,7 @@
         <v>23</v>
       </c>
       <c r="L82">
-        <f>K82-J82</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="M82">
@@ -8587,8 +8816,11 @@
       <c r="AJ82" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK82" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>4</v>
       </c>
@@ -8623,7 +8855,7 @@
         <v>23</v>
       </c>
       <c r="L83">
-        <f>K83-J83</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="M83">
@@ -8677,8 +8909,11 @@
       <c r="AJ83" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK83" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1</v>
       </c>
@@ -8713,7 +8948,7 @@
         <v>26</v>
       </c>
       <c r="L84">
-        <f>K84-J84</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="M84">
@@ -8767,8 +9002,11 @@
       <c r="AJ84" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK84" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2</v>
       </c>
@@ -8803,7 +9041,7 @@
         <v>26</v>
       </c>
       <c r="L85">
-        <f>K85-J85</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="M85">
@@ -8857,8 +9095,11 @@
       <c r="AJ85" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK85" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>3</v>
       </c>
@@ -8893,7 +9134,7 @@
         <v>26</v>
       </c>
       <c r="L86">
-        <f>K86-J86</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="M86">
@@ -8947,8 +9188,11 @@
       <c r="AJ86" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK86" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>4</v>
       </c>
@@ -8983,7 +9227,7 @@
         <v>26</v>
       </c>
       <c r="L87">
-        <f>K87-J87</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="M87">
@@ -9037,8 +9281,11 @@
       <c r="AJ87" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK87" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1</v>
       </c>
@@ -9070,7 +9317,7 @@
         <v>31</v>
       </c>
       <c r="L88">
-        <f>K88-J88</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="M88">
@@ -9124,8 +9371,11 @@
       <c r="AJ88" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK88" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2</v>
       </c>
@@ -9157,7 +9407,7 @@
         <v>31</v>
       </c>
       <c r="L89">
-        <f>K89-J89</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="M89">
@@ -9211,8 +9461,11 @@
       <c r="AJ89" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK89" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="90" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1</v>
       </c>
@@ -9244,7 +9497,7 @@
         <v>31</v>
       </c>
       <c r="L90">
-        <f>K90-J90</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="M90">
@@ -9298,8 +9551,11 @@
       <c r="AJ90" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK90" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="91" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2</v>
       </c>
@@ -9331,7 +9587,7 @@
         <v>31</v>
       </c>
       <c r="L91">
-        <f>K91-J91</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="M91">
@@ -9385,8 +9641,11 @@
       <c r="AJ91" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK91" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="92" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>3</v>
       </c>
@@ -9418,7 +9677,7 @@
         <v>31</v>
       </c>
       <c r="L92">
-        <f>K92-J92</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="M92">
@@ -9472,8 +9731,11 @@
       <c r="AJ92" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK92" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="93" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1</v>
       </c>
@@ -9505,7 +9767,7 @@
         <v>30</v>
       </c>
       <c r="L93">
-        <f>K93-J93</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="M93">
@@ -9559,8 +9821,11 @@
       <c r="AJ93" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK93" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="94" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2</v>
       </c>
@@ -9592,7 +9857,7 @@
         <v>30</v>
       </c>
       <c r="L94">
-        <f>K94-J94</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="M94">
@@ -9646,8 +9911,11 @@
       <c r="AJ94" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK94" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="95" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>3</v>
       </c>
@@ -9679,7 +9947,7 @@
         <v>30</v>
       </c>
       <c r="L95">
-        <f>K95-J95</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="M95">
@@ -9733,8 +10001,11 @@
       <c r="AJ95" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK95" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="96" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>4</v>
       </c>
@@ -9766,7 +10037,7 @@
         <v>30</v>
       </c>
       <c r="L96">
-        <f>K96-J96</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="M96">
@@ -9820,8 +10091,11 @@
       <c r="AJ96" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK96" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="97" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>5</v>
       </c>
@@ -9853,7 +10127,7 @@
         <v>30</v>
       </c>
       <c r="L97">
-        <f>K97-J97</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="M97">
@@ -9907,8 +10181,11 @@
       <c r="AJ97" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK97" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="98" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>6</v>
       </c>
@@ -9940,7 +10217,7 @@
         <v>30</v>
       </c>
       <c r="L98">
-        <f>K98-J98</f>
+        <f t="shared" ref="L98:L129" si="3">K98-J98</f>
         <v>6</v>
       </c>
       <c r="M98">
@@ -9994,8 +10271,11 @@
       <c r="AJ98" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK98" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="99" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>7</v>
       </c>
@@ -10027,7 +10307,7 @@
         <v>30</v>
       </c>
       <c r="L99">
-        <f>K99-J99</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="M99">
@@ -10081,8 +10361,11 @@
       <c r="AJ99" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK99" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="100" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>8</v>
       </c>
@@ -10114,7 +10397,7 @@
         <v>30</v>
       </c>
       <c r="L100">
-        <f>K100-J100</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="M100">
@@ -10168,8 +10451,11 @@
       <c r="AJ100" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK100" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>9</v>
       </c>
@@ -10201,7 +10487,7 @@
         <v>30</v>
       </c>
       <c r="L101">
-        <f>K101-J101</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="M101">
@@ -10255,8 +10541,11 @@
       <c r="AJ101" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK101" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="102" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>10</v>
       </c>
@@ -10288,7 +10577,7 @@
         <v>30</v>
       </c>
       <c r="L102">
-        <f>K102-J102</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="M102">
@@ -10342,8 +10631,11 @@
       <c r="AJ102" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK102" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="103" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>1</v>
       </c>
@@ -10375,7 +10667,7 @@
         <v>32</v>
       </c>
       <c r="L103">
-        <f>K103-J103</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M103">
@@ -10429,8 +10721,11 @@
       <c r="AJ103" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK103" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="104" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2</v>
       </c>
@@ -10462,7 +10757,7 @@
         <v>32</v>
       </c>
       <c r="L104">
-        <f>K104-J104</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M104">
@@ -10516,8 +10811,11 @@
       <c r="AJ104" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK104" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="105" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>3</v>
       </c>
@@ -10549,7 +10847,7 @@
         <v>32</v>
       </c>
       <c r="L105">
-        <f>K105-J105</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M105">
@@ -10603,8 +10901,11 @@
       <c r="AJ105" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK105" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="106" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>4</v>
       </c>
@@ -10636,7 +10937,7 @@
         <v>32</v>
       </c>
       <c r="L106">
-        <f>K106-J106</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M106">
@@ -10690,8 +10991,11 @@
       <c r="AJ106" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK106" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="107" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>5</v>
       </c>
@@ -10723,7 +11027,7 @@
         <v>32</v>
       </c>
       <c r="L107">
-        <f>K107-J107</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M107">
@@ -10777,8 +11081,11 @@
       <c r="AJ107" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK107" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="108" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>6</v>
       </c>
@@ -10810,7 +11117,7 @@
         <v>32</v>
       </c>
       <c r="L108">
-        <f>K108-J108</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M108">
@@ -10864,8 +11171,11 @@
       <c r="AJ108" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK108" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="109" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>7</v>
       </c>
@@ -10897,7 +11207,7 @@
         <v>32</v>
       </c>
       <c r="L109">
-        <f>K109-J109</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M109">
@@ -10951,8 +11261,11 @@
       <c r="AJ109" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK109" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="110" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>8</v>
       </c>
@@ -10984,7 +11297,7 @@
         <v>32</v>
       </c>
       <c r="L110">
-        <f>K110-J110</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M110">
@@ -11038,8 +11351,11 @@
       <c r="AJ110" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK110" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="111" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>9</v>
       </c>
@@ -11071,7 +11387,7 @@
         <v>32</v>
       </c>
       <c r="L111">
-        <f>K111-J111</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M111">
@@ -11125,8 +11441,11 @@
       <c r="AJ111" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK111" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="112" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>10</v>
       </c>
@@ -11158,7 +11477,7 @@
         <v>32</v>
       </c>
       <c r="L112">
-        <f>K112-J112</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M112">
@@ -11212,8 +11531,11 @@
       <c r="AJ112" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK112" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="113" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>1</v>
       </c>
@@ -11248,7 +11570,7 @@
         <v>32</v>
       </c>
       <c r="L113">
-        <f>K113-J113</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M113">
@@ -11308,8 +11630,11 @@
       <c r="AJ113" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK113" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="114" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>1</v>
       </c>
@@ -11344,7 +11669,7 @@
         <v>32</v>
       </c>
       <c r="L114">
-        <f>K114-J114</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M114">
@@ -11404,8 +11729,11 @@
       <c r="AJ114" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK114" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="115" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>1</v>
       </c>
@@ -11440,7 +11768,7 @@
         <v>25</v>
       </c>
       <c r="L115">
-        <f>K115-J115</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M115">
@@ -11500,8 +11828,11 @@
       <c r="AJ115" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK115" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="116" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>1</v>
       </c>
@@ -11536,7 +11867,7 @@
         <v>25</v>
       </c>
       <c r="L116">
-        <f>K116-J116</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M116">
@@ -11596,8 +11927,11 @@
       <c r="AJ116" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK116" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="117" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>1</v>
       </c>
@@ -11632,7 +11966,7 @@
         <v>31.7</v>
       </c>
       <c r="L117">
-        <f>K117-J117</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="M117">
@@ -11692,8 +12026,11 @@
       <c r="AJ117" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK117" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="118" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>1</v>
       </c>
@@ -11728,7 +12065,7 @@
         <v>31.7</v>
       </c>
       <c r="L118">
-        <f>K118-J118</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="M118">
@@ -11788,8 +12125,11 @@
       <c r="AJ118" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK118" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="119" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>2</v>
       </c>
@@ -11824,7 +12164,7 @@
         <v>25</v>
       </c>
       <c r="L119">
-        <f>K119-J119</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M119">
@@ -11884,8 +12224,11 @@
       <c r="AJ119" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK119" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="120" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>2</v>
       </c>
@@ -11920,7 +12263,7 @@
         <v>25</v>
       </c>
       <c r="L120">
-        <f>K120-J120</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="M120">
@@ -11980,8 +12323,11 @@
       <c r="AJ120" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK120" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="121" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>2</v>
       </c>
@@ -12016,7 +12362,7 @@
         <v>31.7</v>
       </c>
       <c r="L121">
-        <f>K121-J121</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="M121">
@@ -12076,8 +12422,11 @@
       <c r="AJ121" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK121" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="122" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>2</v>
       </c>
@@ -12112,7 +12461,7 @@
         <v>31.7</v>
       </c>
       <c r="L122">
-        <f>K122-J122</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="M122">
@@ -12172,8 +12521,11 @@
       <c r="AJ122" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK122" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="123" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>1</v>
       </c>
@@ -12208,7 +12560,7 @@
         <v>14</v>
       </c>
       <c r="L123">
-        <f>K123-J123</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M123">
@@ -12271,8 +12623,11 @@
       <c r="AJ123" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK123" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="124" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>1</v>
       </c>
@@ -12307,7 +12662,7 @@
         <v>23</v>
       </c>
       <c r="L124">
-        <f>K124-J124</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M124">
@@ -12373,8 +12728,11 @@
       <c r="AJ124" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK124" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="125" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>1</v>
       </c>
@@ -12409,7 +12767,7 @@
         <v>30</v>
       </c>
       <c r="L125">
-        <f>K125-J125</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M125">
@@ -12475,8 +12833,11 @@
       <c r="AJ125" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK125" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="126" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>1</v>
       </c>
@@ -12511,7 +12872,7 @@
         <v>14</v>
       </c>
       <c r="L126">
-        <f>K126-J126</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M126">
@@ -12574,8 +12935,11 @@
       <c r="AJ126" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK126" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="127" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>1</v>
       </c>
@@ -12610,7 +12974,7 @@
         <v>23</v>
       </c>
       <c r="L127">
-        <f>K127-J127</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M127">
@@ -12676,8 +13040,11 @@
       <c r="AJ127" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK127" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="128" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>1</v>
       </c>
@@ -12712,7 +13079,7 @@
         <v>30</v>
       </c>
       <c r="L128">
-        <f>K128-J128</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M128">
@@ -12778,8 +13145,11 @@
       <c r="AJ128" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK128" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="129" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>1</v>
       </c>
@@ -12814,7 +13184,7 @@
         <v>14</v>
       </c>
       <c r="L129">
-        <f>K129-J129</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="M129">
@@ -12877,8 +13247,11 @@
       <c r="AJ129" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK129" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="130" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>1</v>
       </c>
@@ -12913,7 +13286,7 @@
         <v>23</v>
       </c>
       <c r="L130">
-        <f>K130-J130</f>
+        <f t="shared" ref="L130:L161" si="4">K130-J130</f>
         <v>14</v>
       </c>
       <c r="M130">
@@ -12979,8 +13352,11 @@
       <c r="AJ130" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK130" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="131" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>1</v>
       </c>
@@ -13015,7 +13391,7 @@
         <v>30</v>
       </c>
       <c r="L131">
-        <f>K131-J131</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M131">
@@ -13081,8 +13457,11 @@
       <c r="AJ131" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK131" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="132" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>1</v>
       </c>
@@ -13117,7 +13496,7 @@
         <v>40</v>
       </c>
       <c r="L132">
-        <f>K132-J132</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M132">
@@ -13183,8 +13562,11 @@
       <c r="AJ132" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK132" s="3" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="133" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>1</v>
       </c>
@@ -13219,7 +13601,7 @@
         <v>14</v>
       </c>
       <c r="L133">
-        <f>K133-J133</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M133">
@@ -13280,8 +13662,11 @@
       <c r="AJ133" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK133" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="134" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>2</v>
       </c>
@@ -13316,7 +13701,7 @@
         <v>23</v>
       </c>
       <c r="L134">
-        <f>K134-J134</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M134">
@@ -13380,8 +13765,11 @@
       <c r="AJ134" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK134" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="135" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>2</v>
       </c>
@@ -13416,7 +13804,7 @@
         <v>30</v>
       </c>
       <c r="L135">
-        <f>K135-J135</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M135">
@@ -13480,8 +13868,11 @@
       <c r="AJ135" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK135" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="136" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>2</v>
       </c>
@@ -13516,7 +13907,7 @@
         <v>40</v>
       </c>
       <c r="L136">
-        <f>K136-J136</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M136">
@@ -13580,8 +13971,11 @@
       <c r="AJ136" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK136" s="3" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="137" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>2</v>
       </c>
@@ -13616,7 +14010,7 @@
         <v>14</v>
       </c>
       <c r="L137">
-        <f>K137-J137</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M137">
@@ -13676,8 +14070,11 @@
       <c r="AJ137" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK137" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="138" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>2</v>
       </c>
@@ -13712,7 +14109,7 @@
         <v>23</v>
       </c>
       <c r="L138">
-        <f>K138-J138</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M138">
@@ -13772,8 +14169,11 @@
       <c r="AJ138" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK138" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="139" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>2</v>
       </c>
@@ -13808,7 +14208,7 @@
         <v>30</v>
       </c>
       <c r="L139">
-        <f>K139-J139</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M139">
@@ -13862,8 +14262,11 @@
       <c r="AJ139" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK139" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="140" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>2</v>
       </c>
@@ -13898,7 +14301,7 @@
         <v>14</v>
       </c>
       <c r="L140">
-        <f>K140-J140</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M140">
@@ -13958,8 +14361,11 @@
       <c r="AJ140" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK140" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="141" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>2</v>
       </c>
@@ -13994,7 +14400,7 @@
         <v>23</v>
       </c>
       <c r="L141">
-        <f>K141-J141</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M141">
@@ -14051,8 +14457,11 @@
       <c r="AJ141" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK141" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="142" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>2</v>
       </c>
@@ -14087,7 +14496,7 @@
         <v>30</v>
       </c>
       <c r="L142">
-        <f>K142-J142</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M142">
@@ -14147,8 +14556,11 @@
       <c r="AJ142" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK142" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="143" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>2</v>
       </c>
@@ -14183,7 +14595,7 @@
         <v>14</v>
       </c>
       <c r="L143">
-        <f>K143-J143</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M143">
@@ -14240,8 +14652,11 @@
       <c r="AJ143" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK143" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="144" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>2</v>
       </c>
@@ -14276,7 +14691,7 @@
         <v>23</v>
       </c>
       <c r="L144">
-        <f>K144-J144</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M144">
@@ -14336,8 +14751,11 @@
       <c r="AJ144" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK144" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="145" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>2</v>
       </c>
@@ -14372,7 +14790,7 @@
         <v>30</v>
       </c>
       <c r="L145">
-        <f>K145-J145</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M145">
@@ -14429,8 +14847,11 @@
       <c r="AJ145" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK145" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="146" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>2</v>
       </c>
@@ -14465,7 +14886,7 @@
         <v>40</v>
       </c>
       <c r="L146">
-        <f>K146-J146</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M146">
@@ -14522,8 +14943,11 @@
       <c r="AJ146" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK146" s="3" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="147" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>2</v>
       </c>
@@ -14558,7 +14982,7 @@
         <v>14</v>
       </c>
       <c r="L147">
-        <f>K147-J147</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M147">
@@ -14618,8 +15042,11 @@
       <c r="AJ147" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK147" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="148" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>2</v>
       </c>
@@ -14654,7 +15081,7 @@
         <v>23</v>
       </c>
       <c r="L148">
-        <f>K148-J148</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M148">
@@ -14714,8 +15141,11 @@
       <c r="AJ148" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK148" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="149" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>2</v>
       </c>
@@ -14750,7 +15180,7 @@
         <v>30</v>
       </c>
       <c r="L149">
-        <f>K149-J149</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M149">
@@ -14810,8 +15240,11 @@
       <c r="AJ149" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK149" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="150" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>2</v>
       </c>
@@ -14846,7 +15279,7 @@
         <v>40</v>
       </c>
       <c r="L150">
-        <f>K150-J150</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M150">
@@ -14906,8 +15339,11 @@
       <c r="AJ150" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK150" s="3" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="151" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>1</v>
       </c>
@@ -14939,7 +15375,7 @@
         <v>31.7</v>
       </c>
       <c r="L151">
-        <f>K151-J151</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M151">
@@ -14993,8 +15429,11 @@
       <c r="AJ151" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK151" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="152" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>2</v>
       </c>
@@ -15026,7 +15465,7 @@
         <v>31.7</v>
       </c>
       <c r="L152">
-        <f>K152-J152</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M152">
@@ -15080,8 +15519,11 @@
       <c r="AJ152" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK152" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="153" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>1</v>
       </c>
@@ -15116,7 +15558,7 @@
         <v>27</v>
       </c>
       <c r="L153">
-        <f>K153-J153</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M153">
@@ -15170,8 +15612,11 @@
       <c r="AJ153" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK153" s="3" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="154" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>2</v>
       </c>
@@ -15206,7 +15651,7 @@
         <v>27</v>
       </c>
       <c r="L154">
-        <f>K154-J154</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M154">
@@ -15260,8 +15705,11 @@
       <c r="AJ154" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK154" s="3" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="155" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>3</v>
       </c>
@@ -15296,7 +15744,7 @@
         <v>27</v>
       </c>
       <c r="L155">
-        <f>K155-J155</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M155">
@@ -15350,8 +15798,11 @@
       <c r="AJ155" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK155" s="3" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="156" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>1</v>
       </c>
@@ -15386,7 +15837,7 @@
         <v>20</v>
       </c>
       <c r="L156">
-        <f>K156-J156</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M156">
@@ -15440,8 +15891,11 @@
       <c r="AJ156" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK156" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="157" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>2</v>
       </c>
@@ -15476,7 +15930,7 @@
         <v>20</v>
       </c>
       <c r="L157">
-        <f>K157-J157</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M157">
@@ -15530,8 +15984,11 @@
       <c r="AJ157" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="AK157" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="158" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>3</v>
       </c>
@@ -15566,7 +16023,7 @@
         <v>20</v>
       </c>
       <c r="L158">
-        <f>K158-J158</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M158">
@@ -15619,6 +16076,9 @@
       </c>
       <c r="AJ158" s="1" t="s">
         <v>202</v>
+      </c>
+      <c r="AK158" s="3" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated metafor excel file
</commit_message>
<xml_diff>
--- a/shared analysis files /metafor.xlsx
+++ b/shared analysis files /metafor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/shared analysis files /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{301DCB65-9442-384B-B095-1BB3A3F429D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5253226F-1176-DF46-89B1-DE3F4BBA8792}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28820" yWindow="-24920" windowWidth="25220" windowHeight="21480" xr2:uid="{4536B02C-F584-4642-B8E5-0FF5356DC288}"/>
   </bookViews>
@@ -1009,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCFBC2B-929F-FD41-8C91-75842D1EBA74}">
   <dimension ref="A1:AK158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="AK159" sqref="AK159"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding in genus/organisms for Verheyen et al 2020
</commit_message>
<xml_diff>
--- a/shared analysis files /metafor.xlsx
+++ b/shared analysis files /metafor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/shared analysis files /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDB460E-3A42-9D49-9567-3E5EBFA592AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB07E494-ADF0-D84E-B659-A4ACA3142F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-11120" windowWidth="24000" windowHeight="15900" xr2:uid="{4536B02C-F584-4642-B8E5-0FF5356DC288}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2984" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3176" uniqueCount="323">
   <si>
     <t>study_id</t>
   </si>
@@ -989,6 +989,12 @@
   <si>
     <t>Sqrt Cellular energy allocation (CEA)</t>
   </si>
+  <si>
+    <t xml:space="preserve">Ischnura </t>
+  </si>
+  <si>
+    <t>elegans </t>
+  </si>
 </sst>
 </file>
 
@@ -1357,8 +1363,8 @@
   <dimension ref="A1:AK369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S368" sqref="S368:S369"/>
+      <pane ySplit="1" topLeftCell="A330" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N338" sqref="N338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26306,6 +26312,21 @@
       <c r="W274" s="2">
         <v>0</v>
       </c>
+      <c r="X274" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y274" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z274" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA274" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB274" s="2">
+        <v>1</v>
+      </c>
       <c r="AC274" t="s">
         <v>311</v>
       </c>
@@ -26389,6 +26410,21 @@
       <c r="W275" s="2">
         <v>0</v>
       </c>
+      <c r="X275" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y275" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z275" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA275" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB275" s="2">
+        <v>1</v>
+      </c>
       <c r="AC275" t="s">
         <v>311</v>
       </c>
@@ -26472,6 +26508,21 @@
       <c r="W276" s="2">
         <v>0</v>
       </c>
+      <c r="X276" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y276" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z276" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA276" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB276" s="2">
+        <v>1</v>
+      </c>
       <c r="AC276" t="s">
         <v>311</v>
       </c>
@@ -26555,6 +26606,21 @@
       <c r="W277" s="2">
         <v>0</v>
       </c>
+      <c r="X277" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y277" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z277" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA277" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB277" s="2">
+        <v>1</v>
+      </c>
       <c r="AC277" t="s">
         <v>311</v>
       </c>
@@ -26638,6 +26704,21 @@
       <c r="W278" s="2">
         <v>0</v>
       </c>
+      <c r="X278" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y278" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z278" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA278" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB278" s="2">
+        <v>1</v>
+      </c>
       <c r="AC278" t="s">
         <v>311</v>
       </c>
@@ -26721,6 +26802,21 @@
       <c r="W279" s="2">
         <v>0</v>
       </c>
+      <c r="X279" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y279" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z279" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA279" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB279" s="2">
+        <v>1</v>
+      </c>
       <c r="AC279" t="s">
         <v>311</v>
       </c>
@@ -26804,6 +26900,21 @@
       <c r="W280" s="2">
         <v>0</v>
       </c>
+      <c r="X280" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y280" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z280" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA280" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB280" s="2">
+        <v>1</v>
+      </c>
       <c r="AC280" t="s">
         <v>311</v>
       </c>
@@ -26887,6 +26998,21 @@
       <c r="W281" s="2">
         <v>0</v>
       </c>
+      <c r="X281" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y281" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z281" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA281" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB281" s="2">
+        <v>1</v>
+      </c>
       <c r="AC281" t="s">
         <v>311</v>
       </c>
@@ -26970,6 +27096,21 @@
       <c r="W282" s="2">
         <v>0</v>
       </c>
+      <c r="X282" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y282" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z282" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA282" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB282" s="2">
+        <v>1</v>
+      </c>
       <c r="AC282" t="s">
         <v>311</v>
       </c>
@@ -27053,6 +27194,21 @@
       <c r="W283" s="2">
         <v>0</v>
       </c>
+      <c r="X283" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y283" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z283" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA283" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB283" s="2">
+        <v>1</v>
+      </c>
       <c r="AC283" t="s">
         <v>311</v>
       </c>
@@ -27136,6 +27292,21 @@
       <c r="W284" s="2">
         <v>0</v>
       </c>
+      <c r="X284" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y284" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z284" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA284" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB284" s="2">
+        <v>1</v>
+      </c>
       <c r="AC284" t="s">
         <v>311</v>
       </c>
@@ -27219,6 +27390,21 @@
       <c r="W285" s="2">
         <v>0</v>
       </c>
+      <c r="X285" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y285" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z285" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA285" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB285" s="2">
+        <v>1</v>
+      </c>
       <c r="AC285" t="s">
         <v>311</v>
       </c>
@@ -27302,6 +27488,21 @@
       <c r="W286" s="2">
         <v>0</v>
       </c>
+      <c r="X286" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y286" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z286" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA286" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB286" s="2">
+        <v>1</v>
+      </c>
       <c r="AC286" t="s">
         <v>311</v>
       </c>
@@ -27385,6 +27586,21 @@
       <c r="W287" s="2">
         <v>0</v>
       </c>
+      <c r="X287" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y287" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z287" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA287" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB287" s="2">
+        <v>1</v>
+      </c>
       <c r="AC287" t="s">
         <v>311</v>
       </c>
@@ -27468,6 +27684,21 @@
       <c r="W288" s="2">
         <v>0</v>
       </c>
+      <c r="X288" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y288" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z288" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA288" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB288" s="2">
+        <v>1</v>
+      </c>
       <c r="AC288" t="s">
         <v>311</v>
       </c>
@@ -27551,6 +27782,21 @@
       <c r="W289" s="2">
         <v>0</v>
       </c>
+      <c r="X289" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y289" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z289" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA289" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB289" s="2">
+        <v>1</v>
+      </c>
       <c r="AC289" t="s">
         <v>311</v>
       </c>
@@ -27634,6 +27880,21 @@
       <c r="W290" s="2">
         <v>0</v>
       </c>
+      <c r="X290" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y290" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z290" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA290" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB290" s="2">
+        <v>1</v>
+      </c>
       <c r="AC290" t="s">
         <v>311</v>
       </c>
@@ -27717,6 +27978,21 @@
       <c r="W291" s="2">
         <v>0</v>
       </c>
+      <c r="X291" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y291" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z291" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA291" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB291" s="2">
+        <v>1</v>
+      </c>
       <c r="AC291" t="s">
         <v>311</v>
       </c>
@@ -27800,6 +28076,21 @@
       <c r="W292" s="2">
         <v>0</v>
       </c>
+      <c r="X292" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y292" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z292" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA292" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB292" s="2">
+        <v>1</v>
+      </c>
       <c r="AC292" t="s">
         <v>311</v>
       </c>
@@ -27883,6 +28174,21 @@
       <c r="W293" s="2">
         <v>0</v>
       </c>
+      <c r="X293" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y293" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z293" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA293" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB293" s="2">
+        <v>1</v>
+      </c>
       <c r="AC293" t="s">
         <v>311</v>
       </c>
@@ -27966,6 +28272,21 @@
       <c r="W294" s="2">
         <v>0</v>
       </c>
+      <c r="X294" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y294" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z294" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA294" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB294" s="2">
+        <v>1</v>
+      </c>
       <c r="AC294" t="s">
         <v>311</v>
       </c>
@@ -28049,6 +28370,21 @@
       <c r="W295" s="2">
         <v>0</v>
       </c>
+      <c r="X295" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y295" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z295" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA295" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB295" s="2">
+        <v>1</v>
+      </c>
       <c r="AC295" t="s">
         <v>311</v>
       </c>
@@ -28132,6 +28468,21 @@
       <c r="W296" s="2">
         <v>0</v>
       </c>
+      <c r="X296" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y296" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z296" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA296" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB296" s="2">
+        <v>1</v>
+      </c>
       <c r="AC296" t="s">
         <v>311</v>
       </c>
@@ -28215,6 +28566,21 @@
       <c r="W297" s="2">
         <v>0</v>
       </c>
+      <c r="X297" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y297" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z297" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA297" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB297" s="2">
+        <v>1</v>
+      </c>
       <c r="AC297" t="s">
         <v>311</v>
       </c>
@@ -28298,6 +28664,21 @@
       <c r="W298" s="2">
         <v>0</v>
       </c>
+      <c r="X298" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y298" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z298" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA298" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB298" s="2">
+        <v>1</v>
+      </c>
       <c r="AC298" t="s">
         <v>311</v>
       </c>
@@ -28381,6 +28762,21 @@
       <c r="W299" s="2">
         <v>0</v>
       </c>
+      <c r="X299" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y299" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z299" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA299" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB299" s="2">
+        <v>1</v>
+      </c>
       <c r="AC299" t="s">
         <v>311</v>
       </c>
@@ -28464,6 +28860,21 @@
       <c r="W300" s="2">
         <v>0</v>
       </c>
+      <c r="X300" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y300" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z300" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA300" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB300" s="2">
+        <v>1</v>
+      </c>
       <c r="AC300" t="s">
         <v>311</v>
       </c>
@@ -28547,6 +28958,21 @@
       <c r="W301" s="2">
         <v>0</v>
       </c>
+      <c r="X301" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y301" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z301" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA301" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB301" s="2">
+        <v>1</v>
+      </c>
       <c r="AC301" t="s">
         <v>311</v>
       </c>
@@ -28630,6 +29056,21 @@
       <c r="W302" s="2">
         <v>0</v>
       </c>
+      <c r="X302" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y302" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z302" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA302" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB302" s="2">
+        <v>1</v>
+      </c>
       <c r="AC302" t="s">
         <v>311</v>
       </c>
@@ -28713,6 +29154,21 @@
       <c r="W303" s="2">
         <v>0</v>
       </c>
+      <c r="X303" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y303" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z303" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA303" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB303" s="2">
+        <v>1</v>
+      </c>
       <c r="AC303" t="s">
         <v>311</v>
       </c>
@@ -28796,6 +29252,21 @@
       <c r="W304" s="2">
         <v>0</v>
       </c>
+      <c r="X304" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y304" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z304" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA304" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB304" s="2">
+        <v>1</v>
+      </c>
       <c r="AC304" t="s">
         <v>311</v>
       </c>
@@ -28879,6 +29350,21 @@
       <c r="W305" s="2">
         <v>0</v>
       </c>
+      <c r="X305" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y305" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z305" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA305" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB305" s="2">
+        <v>1</v>
+      </c>
       <c r="AC305" t="s">
         <v>311</v>
       </c>
@@ -28962,6 +29448,21 @@
       <c r="W306" s="2">
         <v>0</v>
       </c>
+      <c r="X306" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y306" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z306" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA306" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB306" s="2">
+        <v>1</v>
+      </c>
       <c r="AC306" t="s">
         <v>311</v>
       </c>
@@ -29045,6 +29546,21 @@
       <c r="W307" s="2">
         <v>0</v>
       </c>
+      <c r="X307" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y307" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z307" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA307" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB307" s="2">
+        <v>1</v>
+      </c>
       <c r="AC307" t="s">
         <v>311</v>
       </c>
@@ -29128,6 +29644,21 @@
       <c r="W308" s="2">
         <v>0</v>
       </c>
+      <c r="X308" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y308" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z308" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA308" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB308" s="2">
+        <v>1</v>
+      </c>
       <c r="AC308" t="s">
         <v>311</v>
       </c>
@@ -29211,6 +29742,21 @@
       <c r="W309" s="2">
         <v>0</v>
       </c>
+      <c r="X309" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y309" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z309" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA309" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB309" s="2">
+        <v>1</v>
+      </c>
       <c r="AC309" t="s">
         <v>311</v>
       </c>
@@ -29294,6 +29840,21 @@
       <c r="W310" s="2">
         <v>0</v>
       </c>
+      <c r="X310" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y310" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z310" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA310" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB310" s="2">
+        <v>1</v>
+      </c>
       <c r="AC310" t="s">
         <v>311</v>
       </c>
@@ -29377,6 +29938,21 @@
       <c r="W311" s="2">
         <v>0</v>
       </c>
+      <c r="X311" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y311" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z311" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA311" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB311" s="2">
+        <v>1</v>
+      </c>
       <c r="AC311" t="s">
         <v>311</v>
       </c>
@@ -29460,6 +30036,21 @@
       <c r="W312" s="2">
         <v>0</v>
       </c>
+      <c r="X312" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y312" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z312" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA312" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB312" s="2">
+        <v>1</v>
+      </c>
       <c r="AC312" t="s">
         <v>311</v>
       </c>
@@ -29543,6 +30134,21 @@
       <c r="W313" s="2">
         <v>0</v>
       </c>
+      <c r="X313" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y313" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z313" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA313" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB313" s="2">
+        <v>1</v>
+      </c>
       <c r="AC313" t="s">
         <v>311</v>
       </c>
@@ -29626,6 +30232,21 @@
       <c r="W314" s="2">
         <v>0</v>
       </c>
+      <c r="X314" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y314" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z314" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA314" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB314" s="2">
+        <v>1</v>
+      </c>
       <c r="AC314" t="s">
         <v>311</v>
       </c>
@@ -29709,6 +30330,21 @@
       <c r="W315" s="2">
         <v>0</v>
       </c>
+      <c r="X315" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y315" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z315" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA315" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB315" s="2">
+        <v>1</v>
+      </c>
       <c r="AC315" t="s">
         <v>311</v>
       </c>
@@ -29792,6 +30428,21 @@
       <c r="W316" s="2">
         <v>0</v>
       </c>
+      <c r="X316" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y316" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z316" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA316" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB316" s="2">
+        <v>1</v>
+      </c>
       <c r="AC316" t="s">
         <v>311</v>
       </c>
@@ -29875,6 +30526,21 @@
       <c r="W317" s="2">
         <v>0</v>
       </c>
+      <c r="X317" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y317" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z317" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA317" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB317" s="2">
+        <v>1</v>
+      </c>
       <c r="AC317" t="s">
         <v>311</v>
       </c>
@@ -29958,6 +30624,21 @@
       <c r="W318" s="2">
         <v>0</v>
       </c>
+      <c r="X318" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y318" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z318" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA318" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB318" s="2">
+        <v>1</v>
+      </c>
       <c r="AC318" t="s">
         <v>311</v>
       </c>
@@ -30041,6 +30722,21 @@
       <c r="W319" s="2">
         <v>0</v>
       </c>
+      <c r="X319" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y319" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z319" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA319" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB319" s="2">
+        <v>1</v>
+      </c>
       <c r="AC319" t="s">
         <v>311</v>
       </c>
@@ -30124,6 +30820,21 @@
       <c r="W320" s="2">
         <v>0</v>
       </c>
+      <c r="X320" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y320" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z320" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA320" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB320" s="2">
+        <v>1</v>
+      </c>
       <c r="AC320" t="s">
         <v>311</v>
       </c>
@@ -30207,6 +30918,21 @@
       <c r="W321" s="2">
         <v>0</v>
       </c>
+      <c r="X321" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y321" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z321" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA321" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB321" s="2">
+        <v>1</v>
+      </c>
       <c r="AC321" t="s">
         <v>311</v>
       </c>
@@ -30290,6 +31016,21 @@
       <c r="W322" s="2">
         <v>0</v>
       </c>
+      <c r="X322" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y322" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z322" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA322" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB322" s="2">
+        <v>1</v>
+      </c>
       <c r="AC322" t="s">
         <v>311</v>
       </c>
@@ -30373,6 +31114,21 @@
       <c r="W323" s="2">
         <v>0</v>
       </c>
+      <c r="X323" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y323" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z323" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA323" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB323" s="2">
+        <v>1</v>
+      </c>
       <c r="AC323" t="s">
         <v>311</v>
       </c>
@@ -30456,6 +31212,21 @@
       <c r="W324" s="2">
         <v>0</v>
       </c>
+      <c r="X324" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y324" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z324" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA324" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB324" s="2">
+        <v>1</v>
+      </c>
       <c r="AC324" t="s">
         <v>311</v>
       </c>
@@ -30539,6 +31310,21 @@
       <c r="W325" s="2">
         <v>0</v>
       </c>
+      <c r="X325" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y325" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z325" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA325" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB325" s="2">
+        <v>1</v>
+      </c>
       <c r="AC325" t="s">
         <v>311</v>
       </c>
@@ -30622,6 +31408,21 @@
       <c r="W326" s="2">
         <v>0</v>
       </c>
+      <c r="X326" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y326" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z326" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA326" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB326" s="2">
+        <v>1</v>
+      </c>
       <c r="AC326" t="s">
         <v>311</v>
       </c>
@@ -30705,6 +31506,21 @@
       <c r="W327" s="2">
         <v>0</v>
       </c>
+      <c r="X327" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y327" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z327" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA327" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB327" s="2">
+        <v>1</v>
+      </c>
       <c r="AC327" t="s">
         <v>311</v>
       </c>
@@ -30788,6 +31604,21 @@
       <c r="W328" s="2">
         <v>0</v>
       </c>
+      <c r="X328" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y328" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z328" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA328" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB328" s="2">
+        <v>1</v>
+      </c>
       <c r="AC328" t="s">
         <v>311</v>
       </c>
@@ -30871,6 +31702,21 @@
       <c r="W329" s="2">
         <v>0</v>
       </c>
+      <c r="X329" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y329" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z329" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA329" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB329" s="2">
+        <v>1</v>
+      </c>
       <c r="AC329" t="s">
         <v>311</v>
       </c>
@@ -30954,6 +31800,21 @@
       <c r="W330" s="2">
         <v>0</v>
       </c>
+      <c r="X330" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y330" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z330" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA330" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB330" s="2">
+        <v>1</v>
+      </c>
       <c r="AC330" t="s">
         <v>311</v>
       </c>
@@ -31037,6 +31898,21 @@
       <c r="W331" s="2">
         <v>0</v>
       </c>
+      <c r="X331" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y331" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z331" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA331" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB331" s="2">
+        <v>1</v>
+      </c>
       <c r="AC331" t="s">
         <v>311</v>
       </c>
@@ -31120,6 +31996,21 @@
       <c r="W332" s="2">
         <v>0</v>
       </c>
+      <c r="X332" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y332" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z332" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA332" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB332" s="2">
+        <v>1</v>
+      </c>
       <c r="AC332" t="s">
         <v>311</v>
       </c>
@@ -31203,6 +32094,21 @@
       <c r="W333" s="2">
         <v>0</v>
       </c>
+      <c r="X333" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y333" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z333" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA333" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB333" s="2">
+        <v>1</v>
+      </c>
       <c r="AC333" t="s">
         <v>311</v>
       </c>
@@ -31286,6 +32192,21 @@
       <c r="W334" s="2">
         <v>0</v>
       </c>
+      <c r="X334" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y334" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z334" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA334" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB334" s="2">
+        <v>1</v>
+      </c>
       <c r="AC334" t="s">
         <v>311</v>
       </c>
@@ -31369,6 +32290,21 @@
       <c r="W335" s="2">
         <v>0</v>
       </c>
+      <c r="X335" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y335" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z335" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA335" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB335" s="2">
+        <v>1</v>
+      </c>
       <c r="AC335" t="s">
         <v>311</v>
       </c>
@@ -31452,6 +32388,21 @@
       <c r="W336" s="2">
         <v>0</v>
       </c>
+      <c r="X336" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y336" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z336" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA336" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB336" s="2">
+        <v>1</v>
+      </c>
       <c r="AC336" t="s">
         <v>311</v>
       </c>
@@ -31535,6 +32486,21 @@
       <c r="W337" s="2">
         <v>0</v>
       </c>
+      <c r="X337" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y337" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z337" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA337" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB337" s="2">
+        <v>1</v>
+      </c>
       <c r="AC337" t="s">
         <v>311</v>
       </c>
@@ -31615,6 +32581,21 @@
       <c r="W338" s="2">
         <v>0</v>
       </c>
+      <c r="X338" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y338" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z338" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA338" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB338" s="2">
+        <v>1</v>
+      </c>
       <c r="AC338" t="s">
         <v>311</v>
       </c>
@@ -31695,6 +32676,21 @@
       <c r="W339" s="2">
         <v>0</v>
       </c>
+      <c r="X339" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y339" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z339" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA339" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB339" s="2">
+        <v>1</v>
+      </c>
       <c r="AC339" t="s">
         <v>311</v>
       </c>
@@ -31775,6 +32771,21 @@
       <c r="W340" s="2">
         <v>0</v>
       </c>
+      <c r="X340" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y340" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z340" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA340" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB340" s="2">
+        <v>1</v>
+      </c>
       <c r="AC340" t="s">
         <v>311</v>
       </c>
@@ -31855,6 +32866,21 @@
       <c r="W341" s="2">
         <v>0</v>
       </c>
+      <c r="X341" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y341" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z341" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA341" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB341" s="2">
+        <v>1</v>
+      </c>
       <c r="AC341" t="s">
         <v>311</v>
       </c>
@@ -31935,6 +32961,21 @@
       <c r="W342" s="2">
         <v>0</v>
       </c>
+      <c r="X342" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y342" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z342" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA342" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB342" s="2">
+        <v>1</v>
+      </c>
       <c r="AC342" t="s">
         <v>311</v>
       </c>
@@ -32015,6 +33056,21 @@
       <c r="W343" s="2">
         <v>0</v>
       </c>
+      <c r="X343" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y343" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z343" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA343" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB343" s="2">
+        <v>1</v>
+      </c>
       <c r="AC343" t="s">
         <v>311</v>
       </c>
@@ -32095,6 +33151,21 @@
       <c r="W344" s="2">
         <v>0</v>
       </c>
+      <c r="X344" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y344" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z344" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA344" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB344" s="2">
+        <v>1</v>
+      </c>
       <c r="AC344" t="s">
         <v>311</v>
       </c>
@@ -32175,6 +33246,21 @@
       <c r="W345" s="2">
         <v>0</v>
       </c>
+      <c r="X345" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y345" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z345" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA345" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB345" s="2">
+        <v>1</v>
+      </c>
       <c r="AC345" t="s">
         <v>311</v>
       </c>
@@ -32255,6 +33341,21 @@
       <c r="W346" s="2">
         <v>0</v>
       </c>
+      <c r="X346" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y346" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z346" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA346" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB346" s="2">
+        <v>1</v>
+      </c>
       <c r="AC346" t="s">
         <v>311</v>
       </c>
@@ -32335,6 +33436,21 @@
       <c r="W347" s="2">
         <v>0</v>
       </c>
+      <c r="X347" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y347" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z347" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA347" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB347" s="2">
+        <v>1</v>
+      </c>
       <c r="AC347" t="s">
         <v>311</v>
       </c>
@@ -32415,6 +33531,21 @@
       <c r="W348" s="2">
         <v>0</v>
       </c>
+      <c r="X348" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y348" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z348" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA348" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB348" s="2">
+        <v>1</v>
+      </c>
       <c r="AC348" t="s">
         <v>311</v>
       </c>
@@ -32495,6 +33626,21 @@
       <c r="W349" s="2">
         <v>0</v>
       </c>
+      <c r="X349" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y349" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z349" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA349" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB349" s="2">
+        <v>1</v>
+      </c>
       <c r="AC349" t="s">
         <v>311</v>
       </c>
@@ -32575,6 +33721,21 @@
       <c r="W350" s="2">
         <v>0</v>
       </c>
+      <c r="X350" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y350" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z350" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA350" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB350" s="2">
+        <v>1</v>
+      </c>
       <c r="AC350" t="s">
         <v>311</v>
       </c>
@@ -32655,6 +33816,21 @@
       <c r="W351" s="2">
         <v>0</v>
       </c>
+      <c r="X351" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y351" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z351" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA351" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB351" s="2">
+        <v>1</v>
+      </c>
       <c r="AC351" t="s">
         <v>311</v>
       </c>
@@ -32735,6 +33911,21 @@
       <c r="W352" s="2">
         <v>0</v>
       </c>
+      <c r="X352" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y352" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z352" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA352" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB352" s="2">
+        <v>1</v>
+      </c>
       <c r="AC352" t="s">
         <v>311</v>
       </c>
@@ -32815,6 +34006,21 @@
       <c r="W353" s="2">
         <v>0</v>
       </c>
+      <c r="X353" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y353" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z353" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA353" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB353" s="2">
+        <v>1</v>
+      </c>
       <c r="AC353" t="s">
         <v>311</v>
       </c>
@@ -32895,6 +34101,21 @@
       <c r="W354" s="2">
         <v>0</v>
       </c>
+      <c r="X354" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y354" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z354" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA354" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB354" s="2">
+        <v>1</v>
+      </c>
       <c r="AC354" t="s">
         <v>311</v>
       </c>
@@ -32975,6 +34196,21 @@
       <c r="W355" s="2">
         <v>0</v>
       </c>
+      <c r="X355" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y355" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z355" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA355" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB355" s="2">
+        <v>1</v>
+      </c>
       <c r="AC355" t="s">
         <v>311</v>
       </c>
@@ -33055,6 +34291,21 @@
       <c r="W356" s="2">
         <v>0</v>
       </c>
+      <c r="X356" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y356" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z356" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA356" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB356" s="2">
+        <v>1</v>
+      </c>
       <c r="AC356" t="s">
         <v>311</v>
       </c>
@@ -33135,6 +34386,21 @@
       <c r="W357" s="2">
         <v>0</v>
       </c>
+      <c r="X357" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y357" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z357" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA357" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB357" s="2">
+        <v>1</v>
+      </c>
       <c r="AC357" t="s">
         <v>311</v>
       </c>
@@ -33215,6 +34481,21 @@
       <c r="W358" s="2">
         <v>0</v>
       </c>
+      <c r="X358" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y358" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z358" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA358" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB358" s="2">
+        <v>1</v>
+      </c>
       <c r="AC358" t="s">
         <v>311</v>
       </c>
@@ -33295,6 +34576,21 @@
       <c r="W359" s="2">
         <v>0</v>
       </c>
+      <c r="X359" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y359" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z359" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA359" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB359" s="2">
+        <v>1</v>
+      </c>
       <c r="AC359" t="s">
         <v>311</v>
       </c>
@@ -33375,6 +34671,21 @@
       <c r="W360" s="2">
         <v>0</v>
       </c>
+      <c r="X360" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y360" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z360" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA360" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB360" s="2">
+        <v>1</v>
+      </c>
       <c r="AC360" t="s">
         <v>311</v>
       </c>
@@ -33455,6 +34766,21 @@
       <c r="W361" s="2">
         <v>0</v>
       </c>
+      <c r="X361" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y361" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z361" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA361" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB361" s="2">
+        <v>1</v>
+      </c>
       <c r="AC361" t="s">
         <v>311</v>
       </c>
@@ -33535,6 +34861,21 @@
       <c r="W362" s="2">
         <v>0</v>
       </c>
+      <c r="X362" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y362" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z362" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA362" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB362" s="2">
+        <v>1</v>
+      </c>
       <c r="AC362" t="s">
         <v>311</v>
       </c>
@@ -33615,6 +34956,21 @@
       <c r="W363" s="2">
         <v>0</v>
       </c>
+      <c r="X363" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y363" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z363" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA363" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB363" s="2">
+        <v>1</v>
+      </c>
       <c r="AC363" t="s">
         <v>311</v>
       </c>
@@ -33695,6 +35051,21 @@
       <c r="W364" s="2">
         <v>0</v>
       </c>
+      <c r="X364" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y364" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z364" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA364" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB364" s="2">
+        <v>1</v>
+      </c>
       <c r="AC364" t="s">
         <v>311</v>
       </c>
@@ -33775,6 +35146,21 @@
       <c r="W365" s="2">
         <v>0</v>
       </c>
+      <c r="X365" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y365" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z365" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA365" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB365" s="2">
+        <v>1</v>
+      </c>
       <c r="AC365" t="s">
         <v>311</v>
       </c>
@@ -33855,6 +35241,21 @@
       <c r="W366" s="2">
         <v>0</v>
       </c>
+      <c r="X366" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y366" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z366" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA366" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB366" s="2">
+        <v>1</v>
+      </c>
       <c r="AC366" t="s">
         <v>311</v>
       </c>
@@ -33935,6 +35336,21 @@
       <c r="W367" s="2">
         <v>0</v>
       </c>
+      <c r="X367" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y367" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z367" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA367" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB367" s="2">
+        <v>1</v>
+      </c>
       <c r="AC367" t="s">
         <v>311</v>
       </c>
@@ -34015,6 +35431,21 @@
       <c r="W368" s="2">
         <v>0</v>
       </c>
+      <c r="X368" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y368" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z368" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA368" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB368" s="2">
+        <v>1</v>
+      </c>
       <c r="AC368" t="s">
         <v>311</v>
       </c>
@@ -34094,6 +35525,21 @@
       </c>
       <c r="W369" s="2">
         <v>0</v>
+      </c>
+      <c r="X369" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y369" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z369" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA369" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB369" s="2">
+        <v>1</v>
       </c>
       <c r="AC369" t="s">
         <v>311</v>

</xml_diff>